<commit_message>
Work on Logging Framework Fixes #61
</commit_message>
<xml_diff>
--- a/design/NewTablesCentre.xlsx
+++ b/design/NewTablesCentre.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/External HD/matttownsend/Documents/GitHub/mwt-go-dev/design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD2271D-305E-B94B-9751-00676174FF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{957A8937-411E-6C4D-852A-D709F29385C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27180" yWindow="2840" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{D451F61E-BC70-D744-B3AF-222D8D5530A7}"/>
+    <workbookView minimized="1" xWindow="-33820" yWindow="2780" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{D451F61E-BC70-D744-B3AF-222D8D5530A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
     <sheet name="Properties" sheetId="2" r:id="rId2"/>
-    <sheet name="Output" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="datamodel" sheetId="3" r:id="rId3"/>
+    <sheet name="fetchDataCode" sheetId="4" r:id="rId4"/>
+    <sheet name="application" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,95 +39,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>Fields</t>
   </si>
   <si>
-    <t>SienaReference</t>
-  </si>
-  <si>
-    <t>CustomerSienaView</t>
-  </si>
-  <si>
-    <t>SienaCommonRef</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>StartDate</t>
-  </si>
-  <si>
-    <t>MaturityDate</t>
-  </si>
-  <si>
-    <t>ContractNumber</t>
-  </si>
-  <si>
-    <t>ExternalReference</t>
-  </si>
-  <si>
-    <t>CCY</t>
-  </si>
-  <si>
-    <t>Book</t>
-  </si>
-  <si>
-    <t>MandatedUser</t>
-  </si>
-  <si>
-    <t>BackOfficeNotes</t>
-  </si>
-  <si>
-    <t>CashBalance</t>
-  </si>
-  <si>
-    <t>AccountNumber</t>
-  </si>
-  <si>
-    <t>AccountName</t>
-  </si>
-  <si>
-    <t>LedgerBalance</t>
-  </si>
-  <si>
-    <t>Portfolio</t>
-  </si>
-  <si>
-    <t>AgreementId</t>
-  </si>
-  <si>
-    <t>BackOfficeRefNo</t>
-  </si>
-  <si>
-    <t>PaymentSystemSienaView</t>
-  </si>
-  <si>
-    <t>ISIN</t>
-  </si>
-  <si>
-    <t>UTI</t>
-  </si>
-  <si>
-    <t>CCYName</t>
-  </si>
-  <si>
-    <t>BookName</t>
-  </si>
-  <si>
-    <t>PortfolioName</t>
-  </si>
-  <si>
     <t>Centre</t>
   </si>
   <si>
-    <t>Firm</t>
-  </si>
-  <si>
-    <t>CCYDp</t>
-  </si>
-  <si>
     <t>Object</t>
   </si>
   <si>
@@ -167,6 +87,45 @@
   </si>
   <si>
     <t>///</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>CountryName</t>
+  </si>
+  <si>
+    <t>const (</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>SQL Field Types</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Int</t>
+  </si>
+  <si>
+    <t>Float</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>Save</t>
   </si>
 </sst>
 </file>
@@ -525,225 +484,152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3644CAC-10B5-0849-983E-6F28E90ACCA1}">
-  <dimension ref="A1:A29"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="B5" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F514AAB7-5D2C-6240-9A7E-B96993232A80}">
+          <x14:formula1>
+            <xm:f>Properties!$J$3:$J$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B45</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B09CF151-9BAC-7549-8E2D-73C40A4E3050}">
-  <dimension ref="B2:G6"/>
+  <dimension ref="B2:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D4" t="str">
         <f>UPPER(LEFT(C4,1))&amp;RIGHT(C4,LEN(C4)-1)</f>
         <v>Siena</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="J4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="J5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="G6" t="s">
-        <v>38</v>
+        <v>11</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -753,10 +639,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87877DC2-0A1D-B14C-ACD0-0BF8A8D89A4A}">
-  <dimension ref="A2:A45"/>
+  <dimension ref="A1:A45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -764,6 +650,11 @@
     <col min="1" max="1" width="56.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>Properties!C2&amp;"_Title = "&amp;""""&amp;Properties!C3&amp;""""</f>
@@ -784,17 +675,17 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
@@ -823,185 +714,185 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A2&amp;" = "&amp;""""&amp;Fields!A2&amp;""""</f>
-        <v>Centre_SienaReference = "SienaReference"</v>
+        <v>Centre_Code = "Code"</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A3&amp;" = "&amp;""""&amp;Fields!A3&amp;""""</f>
-        <v>Centre_CustomerSienaView = "CustomerSienaView"</v>
+        <v>Centre_Name = "Name"</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A4&amp;" = "&amp;""""&amp;Fields!A4&amp;""""</f>
-        <v>Centre_SienaCommonRef = "SienaCommonRef"</v>
+        <v>Centre_Country = "Country"</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A5&amp;" = "&amp;""""&amp;Fields!A5&amp;""""</f>
-        <v>Centre_Status = "Status"</v>
+        <v>Centre_CountryName = "CountryName"</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A6&amp;" = "&amp;""""&amp;Fields!A6&amp;""""</f>
-        <v>Centre_StartDate = "StartDate"</v>
+        <v>Centre_ = ""</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A7&amp;" = "&amp;""""&amp;Fields!A7&amp;""""</f>
-        <v>Centre_MaturityDate = "MaturityDate"</v>
+        <v>Centre_ = ""</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A8&amp;" = "&amp;""""&amp;Fields!A8&amp;""""</f>
-        <v>Centre_ContractNumber = "ContractNumber"</v>
+        <v>Centre_ = ""</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A9&amp;" = "&amp;""""&amp;Fields!A9&amp;""""</f>
-        <v>Centre_ExternalReference = "ExternalReference"</v>
+        <v>Centre_ = ""</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A10&amp;" = "&amp;""""&amp;Fields!A10&amp;""""</f>
-        <v>Centre_CCY = "CCY"</v>
+        <v>Centre_ = ""</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A11&amp;" = "&amp;""""&amp;Fields!A11&amp;""""</f>
-        <v>Centre_Book = "Book"</v>
+        <v>Centre_ = ""</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A12&amp;" = "&amp;""""&amp;Fields!A12&amp;""""</f>
-        <v>Centre_MandatedUser = "MandatedUser"</v>
+        <v>Centre_ = ""</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A13&amp;" = "&amp;""""&amp;Fields!A13&amp;""""</f>
-        <v>Centre_BackOfficeNotes = "BackOfficeNotes"</v>
+        <v>Centre_ = ""</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A14&amp;" = "&amp;""""&amp;Fields!A14&amp;""""</f>
-        <v>Centre_CashBalance = "CashBalance"</v>
+        <v>Centre_ = ""</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A15&amp;" = "&amp;""""&amp;Fields!A15&amp;""""</f>
-        <v>Centre_AccountNumber = "AccountNumber"</v>
+        <v>Centre_ = ""</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A16&amp;" = "&amp;""""&amp;Fields!A16&amp;""""</f>
-        <v>Centre_AccountName = "AccountName"</v>
+        <v>Centre_ = ""</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A17&amp;" = "&amp;""""&amp;Fields!A17&amp;""""</f>
-        <v>Centre_LedgerBalance = "LedgerBalance"</v>
+        <v>Centre_ = ""</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A18&amp;" = "&amp;""""&amp;Fields!A18&amp;""""</f>
-        <v>Centre_Portfolio = "Portfolio"</v>
+        <v>Centre_ = ""</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A19&amp;" = "&amp;""""&amp;Fields!A19&amp;""""</f>
-        <v>Centre_AgreementId = "AgreementId"</v>
+        <v>Centre_ = ""</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A20&amp;" = "&amp;""""&amp;Fields!A20&amp;""""</f>
-        <v>Centre_BackOfficeRefNo = "BackOfficeRefNo"</v>
+        <v>Centre_ = ""</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A21&amp;" = "&amp;""""&amp;Fields!A21&amp;""""</f>
-        <v>Centre_PaymentSystemSienaView = "PaymentSystemSienaView"</v>
+        <v>Centre_ = ""</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A22&amp;" = "&amp;""""&amp;Fields!A22&amp;""""</f>
-        <v>Centre_ISIN = "ISIN"</v>
+        <v>Centre_ = ""</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A23&amp;" = "&amp;""""&amp;Fields!A23&amp;""""</f>
-        <v>Centre_UTI = "UTI"</v>
+        <v>Centre_ = ""</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A24&amp;" = "&amp;""""&amp;Fields!A24&amp;""""</f>
-        <v>Centre_CCYName = "CCYName"</v>
+        <v>Centre_ = ""</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A25&amp;" = "&amp;""""&amp;Fields!A25&amp;""""</f>
-        <v>Centre_BookName = "BookName"</v>
+        <v>Centre_ = ""</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A26&amp;" = "&amp;""""&amp;Fields!A26&amp;""""</f>
-        <v>Centre_PortfolioName = "PortfolioName"</v>
+        <v>Centre_ = ""</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A27&amp;" = "&amp;""""&amp;Fields!A27&amp;""""</f>
-        <v>Centre_Centre = "Centre"</v>
+        <v>Centre_ = ""</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A28&amp;" = "&amp;""""&amp;Fields!A28&amp;""""</f>
-        <v>Centre_Firm = "Firm"</v>
+        <v>Centre_ = ""</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="str">
         <f>Properties!$C$2&amp;"_"&amp;Fields!A29&amp;" = "&amp;""""&amp;Fields!A29&amp;""""</f>
-        <v>Centre_CCYDp = "CCYDp"</v>
+        <v>Centre_ = ""</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
@@ -1029,12 +920,167 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C1373A-436A-2F48-A706-51C776BAE2E1}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A1:A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="str">
+        <f>Properties!$C$4&amp;Properties!$C$2&amp;"."&amp;Fields!A2&amp;" = get_"&amp;Fields!B2&amp;"(rec, dm."&amp;Properties!$C$2&amp;"_"&amp;Fields!A2&amp;","&amp;""""&amp;""""&amp;")"</f>
+        <v>sienaCentre.Code = get_String(rec, dm.Centre_Code,"")</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>Properties!$C$4&amp;Properties!$C$2&amp;"."&amp;Fields!A3&amp;" = get_"&amp;Fields!B3&amp;"(rec, dm."&amp;Properties!$C$2&amp;"_"&amp;Fields!A3&amp;","&amp;""""&amp;""""&amp;")"</f>
+        <v>sienaCentre.Name = get_String(rec, dm.Centre_Name,"")</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>Properties!$C$4&amp;Properties!$C$2&amp;"."&amp;Fields!A4&amp;" = get_"&amp;Fields!B4&amp;"(rec, dm."&amp;Properties!$C$2&amp;"_"&amp;Fields!A4&amp;","&amp;""""&amp;""""&amp;")"</f>
+        <v>sienaCentre.Country = get_String(rec, dm.Centre_Country,"")</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f>Properties!$C$4&amp;Properties!$C$2&amp;"."&amp;Fields!A5&amp;" = get_"&amp;Fields!B5&amp;"(rec, dm."&amp;Properties!$C$2&amp;"_"&amp;Fields!A5&amp;","&amp;""""&amp;""""&amp;")"</f>
+        <v>sienaCentre.CountryName = get_String(rec, dm.Centre_CountryName,"")</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="str">
+        <f>Properties!$C$4&amp;Properties!$C$2&amp;"."&amp;Fields!A6&amp;" = get_"&amp;Fields!B6&amp;"(rec, dm."&amp;Properties!$C$2&amp;"_"&amp;Fields!A6&amp;","&amp;""""&amp;""""&amp;")"</f>
+        <v>sienaCentre. = get_(rec, dm.Centre_,"")</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="str">
+        <f>Properties!$C$4&amp;Properties!$C$2&amp;"."&amp;Fields!A7&amp;" = get_"&amp;Fields!B7&amp;"(rec, dm."&amp;Properties!$C$2&amp;"_"&amp;Fields!A7&amp;","&amp;""""&amp;""""&amp;")"</f>
+        <v>sienaCentre. = get_(rec, dm.Centre_,"")</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="str">
+        <f>Properties!$C$4&amp;Properties!$C$2&amp;"."&amp;Fields!A8&amp;" = get_"&amp;Fields!B8&amp;"(rec, dm."&amp;Properties!$C$2&amp;"_"&amp;Fields!A8&amp;","&amp;""""&amp;""""&amp;")"</f>
+        <v>sienaCentre. = get_(rec, dm.Centre_,"")</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="str">
+        <f>Properties!$C$4&amp;Properties!$C$2&amp;"."&amp;Fields!A9&amp;" = get_"&amp;Fields!B9&amp;"(rec, dm."&amp;Properties!$C$2&amp;"_"&amp;Fields!A9&amp;","&amp;""""&amp;""""&amp;")"</f>
+        <v>sienaCentre. = get_(rec, dm.Centre_,"")</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="str">
+        <f>Properties!$C$4&amp;Properties!$C$2&amp;"."&amp;Fields!A10&amp;" = get_"&amp;Fields!B10&amp;"(rec, dm."&amp;Properties!$C$2&amp;"_"&amp;Fields!A10&amp;","&amp;""""&amp;""""&amp;")"</f>
+        <v>sienaCentre. = get_(rec, dm.Centre_,"")</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="str">
+        <f>Properties!$C$4&amp;Properties!$C$2&amp;"."&amp;Fields!A11&amp;" = get_"&amp;Fields!B11&amp;"(rec, dm."&amp;Properties!$C$2&amp;"_"&amp;Fields!A11&amp;","&amp;""""&amp;""""&amp;")"</f>
+        <v>sienaCentre. = get_(rec, dm.Centre_,"")</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="str">
+        <f>Properties!$C$4&amp;Properties!$C$2&amp;"."&amp;Fields!A12&amp;" = get_"&amp;Fields!B12&amp;"(rec, dm."&amp;Properties!$C$2&amp;"_"&amp;Fields!A12&amp;","&amp;""""&amp;""""&amp;")"</f>
+        <v>sienaCentre. = get_(rec, dm.Centre_,"")</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="str">
+        <f>Properties!$C$4&amp;Properties!$C$2&amp;"."&amp;Fields!A13&amp;" = get_"&amp;Fields!B13&amp;"(rec, dm."&amp;Properties!$C$2&amp;"_"&amp;Fields!A13&amp;","&amp;""""&amp;""""&amp;")"</f>
+        <v>sienaCentre. = get_(rec, dm.Centre_,"")</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="str">
+        <f>Properties!$C$4&amp;Properties!$C$2&amp;"."&amp;Fields!A14&amp;" = get_"&amp;Fields!B14&amp;"(rec, dm."&amp;Properties!$C$2&amp;"_"&amp;Fields!A14&amp;","&amp;""""&amp;""""&amp;")"</f>
+        <v>sienaCentre. = get_(rec, dm.Centre_,"")</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="str">
+        <f>Properties!$C$4&amp;Properties!$C$2&amp;"."&amp;Fields!A15&amp;" = get_"&amp;Fields!B15&amp;"(rec, dm."&amp;Properties!$C$2&amp;"_"&amp;Fields!A15&amp;","&amp;""""&amp;""""&amp;")"</f>
+        <v>sienaCentre. = get_(rec, dm.Centre_,"")</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="str">
+        <f>Properties!$C$4&amp;Properties!$C$2&amp;"."&amp;Fields!A16&amp;" = get_"&amp;Fields!B16&amp;"(rec, dm."&amp;Properties!$C$2&amp;"_"&amp;Fields!A16&amp;","&amp;""""&amp;""""&amp;")"</f>
+        <v>sienaCentre. = get_(rec, dm.Centre_,"")</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8405935-2100-3A48-99FD-4D95018F9863}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A1:A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="str">
+        <f>"func "&amp;Properties!C2&amp;"_Publish(mux http.ServeMux){"</f>
+        <v>func Centre_Publish(mux http.ServeMux){</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>"mux.HandleFunc("&amp;""""&amp;"/"&amp;LOWER(Properties!G3)&amp;Properties!$D$4&amp;Properties!$C$2&amp;"/"&amp;""""&amp;","&amp;Properties!$C$2&amp;"_Handler"&amp;Properties!G3&amp;")"</f>
+        <v>mux.HandleFunc("/listSienaCentre/",Centre_HandlerList)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>"mux.HandleFunc("&amp;""""&amp;"/"&amp;LOWER(Properties!G4)&amp;Properties!$D$4&amp;Properties!$C$2&amp;"/"&amp;""""&amp;","&amp;Properties!$C$2&amp;"_Handler"&amp;Properties!G4&amp;")"</f>
+        <v>mux.HandleFunc("/viewSienaCentre/",Centre_HandlerView)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f>"mux.HandleFunc("&amp;""""&amp;"/"&amp;LOWER(Properties!G5)&amp;Properties!$D$4&amp;Properties!$C$2&amp;"/"&amp;""""&amp;","&amp;Properties!$C$2&amp;"_Handler"&amp;Properties!G5&amp;")"</f>
+        <v>mux.HandleFunc("/editSienaCentre/",Centre_HandlerEdit)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="str">
+        <f>"mux.HandleFunc("&amp;""""&amp;"/"&amp;LOWER(Properties!G6)&amp;Properties!$D$4&amp;Properties!$C$2&amp;"/"&amp;""""&amp;","&amp;Properties!$C$2&amp;"_Handler"&amp;Properties!G6&amp;")"</f>
+        <v>mux.HandleFunc("/newSienaCentre/",Centre_HandlerNew)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="str">
+        <f>"mux.HandleFunc("&amp;""""&amp;"/"&amp;LOWER(Properties!G7)&amp;Properties!$D$4&amp;Properties!$C$2&amp;"/"&amp;""""&amp;","&amp;Properties!$C$2&amp;"_Handler"&amp;Properties!G7&amp;")"</f>
+        <v>mux.HandleFunc("/saveSienaCentre/",Centre_HandlerSave)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="str">
+        <f>"core.LOG_mux("&amp;""""&amp;Properties!D5&amp;""""&amp;", dm."&amp;Properties!C3&amp;"_Title)"</f>
+        <v>core.LOG_mux("", dm.Centre_Title)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>